<commit_message>
added 'import bone_morphs' functionality added eyes controller bone
</commit_message>
<xml_diff>
--- a/ffxiv_mmd_tools_helper_beta/data/joint.xlsx
+++ b/ffxiv_mmd_tools_helper_beta/data/joint.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MMD\ffxiv_mmd_tools_helper\ffxiv_mmd_tools_helper_beta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D13C7C-2EA5-429D-8DF0-39871E33F7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90173F1A-D9AF-416F-9902-3ACA0152FA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47040" yWindow="4035" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
   <si>
     <t>head</t>
   </si>
@@ -118,6 +119,78 @@
   </si>
   <si>
     <t>j_kami_f_r</t>
+  </si>
+  <si>
+    <t>n_sippo_a</t>
+  </si>
+  <si>
+    <t>n_sippo_b</t>
+  </si>
+  <si>
+    <t>n_sippo_c</t>
+  </si>
+  <si>
+    <t>n_sippo_d</t>
+  </si>
+  <si>
+    <t>n_sippo_e</t>
+  </si>
+  <si>
+    <t>lower body</t>
+  </si>
+  <si>
+    <t>j_sk_b_a_l</t>
+  </si>
+  <si>
+    <t>j_sk_b_a_r</t>
+  </si>
+  <si>
+    <t>j_sk_b_b_l</t>
+  </si>
+  <si>
+    <t>j_sk_b_b_r</t>
+  </si>
+  <si>
+    <t>j_sk_b_c_l</t>
+  </si>
+  <si>
+    <t>j_sk_b_c_r</t>
+  </si>
+  <si>
+    <t>j_sk_f_a_l</t>
+  </si>
+  <si>
+    <t>j_sk_f_a_r</t>
+  </si>
+  <si>
+    <t>j_sk_f_b_l</t>
+  </si>
+  <si>
+    <t>j_sk_f_b_r</t>
+  </si>
+  <si>
+    <t>j_sk_f_c_l</t>
+  </si>
+  <si>
+    <t>j_sk_f_c_r</t>
+  </si>
+  <si>
+    <t>j_sk_s_a_l</t>
+  </si>
+  <si>
+    <t>j_sk_s_a_r</t>
+  </si>
+  <si>
+    <t>j_sk_s_b_l</t>
+  </si>
+  <si>
+    <t>j_sk_s_b_r</t>
+  </si>
+  <si>
+    <t>j_sk_s_c_l</t>
+  </si>
+  <si>
+    <t>j_sk_s_c_r</t>
   </si>
 </sst>
 </file>
@@ -141,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,8 +227,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -172,15 +251,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,8 +340,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{986ADBC9-5641-4E2C-BC2D-3201D64FDDC8}" name="Table22" displayName="Table22" ref="A1:U9" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:U9" xr:uid="{986ADBC9-5641-4E2C-BC2D-3201D64FDDC8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{986ADBC9-5641-4E2C-BC2D-3201D64FDDC8}" name="Table22" displayName="Table22" ref="A1:U50" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:U50" xr:uid="{986ADBC9-5641-4E2C-BC2D-3201D64FDDC8}"/>
   <tableColumns count="21">
     <tableColumn id="6" xr3:uid="{46085F6A-14DA-41C2-880B-EA29369D9E3D}" name="rigid_body_child"/>
     <tableColumn id="3" xr3:uid="{E619AE08-CCC5-4E49-92F3-B342CA7A97F8}" name="rigid_body_parent"/>
@@ -523,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D213BE9-EC88-43A5-B10E-7AC8A26A2FF6}">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,10 +964,887 @@
         <v>5</v>
       </c>
     </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>-5</v>
+      </c>
+      <c r="K10">
+        <v>-5</v>
+      </c>
+      <c r="L10">
+        <v>-5</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>-15</v>
+      </c>
+      <c r="K11">
+        <v>-15</v>
+      </c>
+      <c r="L11">
+        <v>-15</v>
+      </c>
+      <c r="M11">
+        <v>15</v>
+      </c>
+      <c r="N11">
+        <v>15</v>
+      </c>
+      <c r="O11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>-15</v>
+      </c>
+      <c r="K12">
+        <v>-15</v>
+      </c>
+      <c r="L12">
+        <v>-15</v>
+      </c>
+      <c r="M12">
+        <v>15</v>
+      </c>
+      <c r="N12">
+        <v>15</v>
+      </c>
+      <c r="O12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>-15</v>
+      </c>
+      <c r="K13">
+        <v>-15</v>
+      </c>
+      <c r="L13">
+        <v>-15</v>
+      </c>
+      <c r="M13">
+        <v>15</v>
+      </c>
+      <c r="N13">
+        <v>15</v>
+      </c>
+      <c r="O13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>-15</v>
+      </c>
+      <c r="K14">
+        <v>-15</v>
+      </c>
+      <c r="L14">
+        <v>-15</v>
+      </c>
+      <c r="M14">
+        <v>15</v>
+      </c>
+      <c r="N14">
+        <v>15</v>
+      </c>
+      <c r="O14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J33" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K33">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J34" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K34">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J35" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K35">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J36" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K36">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J37" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K37">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J38" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K38">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J39" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K39">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J40" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K40">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K41">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J42" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K42">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J43" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K43">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J44" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K44">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J45" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K45">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J46" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K46">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J47" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K47">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J48" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K48">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J49" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K49">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J50" s="7">
+        <v>-5.3100000000000001E-2</v>
+      </c>
+      <c r="K50">
+        <v>5.3100000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02AA316-0263-424B-8ABD-34C5FBB0BE1E}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>